<commit_message>
Update planning with additional date
</commit_message>
<xml_diff>
--- a/Cours/cours1/planning_dsp_2026-02.xlsx
+++ b/Cours/cours1/planning_dsp_2026-02.xlsx
@@ -11,7 +11,7 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$D$13</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">Sheet1!$A$1:$D$14</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="13">
   <si>
     <t xml:space="preserve">Date</t>
   </si>
@@ -70,7 +70,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="dd/mm/yy"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
     <numFmt numFmtId="166" formatCode="h:mm"/>
   </numFmts>
   <fonts count="5">
@@ -120,13 +120,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.3999"/>
+        <fgColor theme="7" tint="0.3998"/>
         <bgColor rgb="FFF4B183"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.3999"/>
+        <fgColor theme="5" tint="0.3998"/>
         <bgColor rgb="FFFFD966"/>
       </patternFill>
     </fill>
@@ -500,13 +500,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A13"/>
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.71484375" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="1" style="0" width="10.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.15"/>
@@ -528,7 +528,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="n">
-        <v>46079</v>
+        <v>46078</v>
       </c>
       <c r="B2" s="3" t="n">
         <v>0.375</v>
@@ -545,7 +545,7 @@
         <v>46079</v>
       </c>
       <c r="B3" s="7" t="n">
-        <v>0.5625</v>
+        <v>0.375</v>
       </c>
       <c r="C3" s="8" t="s">
         <v>6</v>
@@ -556,10 +556,10 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="n">
-        <v>46085</v>
+        <v>46079</v>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.375</v>
+        <v>0.5625</v>
       </c>
       <c r="C4" s="4" t="s">
         <v>4</v>
@@ -573,7 +573,7 @@
         <v>46085</v>
       </c>
       <c r="B5" s="7" t="n">
-        <v>0.5625</v>
+        <v>0.375</v>
       </c>
       <c r="C5" s="8" t="s">
         <v>6</v>
@@ -584,10 +584,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
-        <v>46087</v>
+        <v>46085</v>
       </c>
       <c r="B6" s="3" t="n">
-        <v>0.375</v>
+        <v>0.5625</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>4</v>
@@ -601,7 +601,7 @@
         <v>46087</v>
       </c>
       <c r="B7" s="7" t="n">
-        <v>0.5625</v>
+        <v>0.375</v>
       </c>
       <c r="C7" s="8" t="s">
         <v>6</v>
@@ -611,30 +611,30 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="n">
+      <c r="A8" s="6" t="n">
+        <v>46087</v>
+      </c>
+      <c r="B8" s="7" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
         <v>46092</v>
       </c>
-      <c r="B8" s="3" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="C8" s="4" t="s">
+      <c r="B9" s="3" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="6" t="n">
-        <v>46094</v>
-      </c>
-      <c r="B9" s="7" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="C9" s="8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="5" t="s">
         <v>9</v>
       </c>
     </row>
@@ -643,7 +643,7 @@
         <v>46094</v>
       </c>
       <c r="B10" s="7" t="n">
-        <v>0.5625</v>
+        <v>0.375</v>
       </c>
       <c r="C10" s="8" t="s">
         <v>6</v>
@@ -653,22 +653,22 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="10" t="n">
-        <v>46099</v>
-      </c>
-      <c r="B11" s="11" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="C11" s="12" t="s">
+      <c r="A11" s="6" t="n">
+        <v>46094</v>
+      </c>
+      <c r="B11" s="7" t="n">
+        <v>0.5625</v>
+      </c>
+      <c r="C11" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>10</v>
+      <c r="D11" s="9" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="n">
-        <v>46101</v>
+        <v>46099</v>
       </c>
       <c r="B12" s="11" t="n">
         <v>0.375</v>
@@ -681,16 +681,30 @@
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="14" t="n">
+      <c r="A13" s="10" t="n">
+        <v>46101</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C13" s="12" t="s">
+        <v>6</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="n">
         <v>46106</v>
       </c>
-      <c r="B13" s="15" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="C13" s="16" t="s">
+      <c r="B14" s="15" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="C14" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="D14" s="17" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>